<commit_message>
Changed some windows to dialogs , enhanced UI/UX
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="868" firstSheet="5" activeTab="10" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="868" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="المناسبات" sheetId="1" state="visible" r:id="rId1"/>
@@ -1120,8 +1120,8 @@
   </sheetPr>
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="17.85546875" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -1139,8 +1139,8 @@
     <col width="11.140625" customWidth="1" style="6" min="11" max="11"/>
     <col width="17.85546875" customWidth="1" style="6" min="12" max="12"/>
     <col width="28" customWidth="1" style="6" min="13" max="13"/>
-    <col width="17.85546875" customWidth="1" style="6" min="14" max="75"/>
-    <col width="17.85546875" customWidth="1" style="6" min="76" max="16384"/>
+    <col width="17.85546875" customWidth="1" style="6" min="14" max="76"/>
+    <col width="17.85546875" customWidth="1" style="6" min="77" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="23.25" customHeight="1" s="51">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="G4" s="41" t="inlineStr">
         <is>
-          <t xml:space="preserve">برمون الميلاد </t>
+          <t>برمون الميلاد</t>
         </is>
       </c>
       <c r="I4" s="28" t="n">
@@ -1329,7 +1329,7 @@
       </c>
       <c r="G5" s="41" t="inlineStr">
         <is>
-          <t xml:space="preserve">الميلاد </t>
+          <t>الميلاد</t>
         </is>
       </c>
       <c r="I5" s="28" t="n">
@@ -2300,7 +2300,7 @@
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
@@ -7895,7 +7895,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="53" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -7906,13 +7906,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="53" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="53" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="53" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -7923,13 +7923,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="53" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" s="53" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" s="53" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
@@ -7940,13 +7940,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="53" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5" s="53" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E5" s="53" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
@@ -7957,13 +7957,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="53" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" s="53" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E6" s="53" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7">
@@ -7974,13 +7974,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="53" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D7" s="53" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E7" s="53" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8">
@@ -7991,13 +7991,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="53" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D8" s="53" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E8" s="53" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
@@ -8008,13 +8008,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="53" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D9" s="53" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E9" s="53" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
@@ -8025,13 +8025,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="53" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D10" s="53" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E10" s="53" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11">
@@ -8042,13 +8042,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="53" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D11" s="53" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E11" s="53" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12">
@@ -8059,13 +8059,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="53" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D12" s="53" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E12" s="53" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13">
@@ -8076,13 +8076,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="53" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D13" s="53" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E13" s="53" t="n">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14">
@@ -8093,13 +8093,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="53" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D14" s="53" t="n">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E14" s="53" t="n">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15">
@@ -8110,13 +8110,13 @@
         <v>3</v>
       </c>
       <c r="C15" s="53" t="n">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D15" s="53" t="n">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E15" s="53" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16">
@@ -8127,13 +8127,13 @@
         <v>3</v>
       </c>
       <c r="C16" s="53" t="n">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D16" s="53" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E16" s="53" t="n">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17">
@@ -8144,13 +8144,13 @@
         <v>3</v>
       </c>
       <c r="C17" s="53" t="n">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D17" s="53" t="n">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E17" s="53" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18">
@@ -8161,13 +8161,13 @@
         <v>3</v>
       </c>
       <c r="C18" s="53" t="n">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D18" s="53" t="n">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E18" s="53" t="n">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19">
@@ -8178,13 +8178,13 @@
         <v>3</v>
       </c>
       <c r="C19" s="53" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D19" s="53" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E19" s="53" t="n">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20">
@@ -8195,13 +8195,13 @@
         <v>3</v>
       </c>
       <c r="C20" s="53" t="n">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D20" s="53" t="n">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E20" s="53" t="n">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21">
@@ -8212,13 +8212,13 @@
         <v>3</v>
       </c>
       <c r="C21" s="53" t="n">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D21" s="53" t="n">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E21" s="53" t="n">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22">
@@ -8229,13 +8229,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="53" t="n">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D22" s="53" t="n">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E22" s="53" t="n">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23">
@@ -8246,13 +8246,13 @@
         <v>3</v>
       </c>
       <c r="C23" s="53" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D23" s="53" t="n">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E23" s="53" t="n">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24">
@@ -8263,13 +8263,13 @@
         <v>3</v>
       </c>
       <c r="C24" s="53" t="n">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D24" s="53" t="n">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E24" s="53" t="n">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25">
@@ -8280,13 +8280,13 @@
         <v>3</v>
       </c>
       <c r="C25" s="53" t="n">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D25" s="53" t="n">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E25" s="53" t="n">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26">
@@ -8297,13 +8297,13 @@
         <v>4</v>
       </c>
       <c r="C26" s="53" t="n">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D26" s="53" t="n">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E26" s="53" t="n">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27">
@@ -8314,13 +8314,13 @@
         <v>4</v>
       </c>
       <c r="C27" s="53" t="n">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D27" s="53" t="n">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E27" s="53" t="n">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28">
@@ -8331,13 +8331,13 @@
         <v>4</v>
       </c>
       <c r="C28" s="53" t="n">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D28" s="53" t="n">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E28" s="53" t="n">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="29">
@@ -8348,13 +8348,13 @@
         <v>4</v>
       </c>
       <c r="C29" s="53" t="n">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D29" s="53" t="n">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E29" s="53" t="n">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30">
@@ -8365,13 +8365,13 @@
         <v>4</v>
       </c>
       <c r="C30" s="53" t="n">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D30" s="53" t="n">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E30" s="53" t="n">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="31">
@@ -8382,13 +8382,13 @@
         <v>5</v>
       </c>
       <c r="C31" s="53" t="n">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D31" s="53" t="n">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E31" s="53" t="n">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="32">
@@ -8399,13 +8399,13 @@
         <v>5</v>
       </c>
       <c r="C32" s="53" t="n">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D32" s="53" t="n">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E32" s="53" t="n">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33">
@@ -8416,13 +8416,13 @@
         <v>5</v>
       </c>
       <c r="C33" s="53" t="n">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D33" s="53" t="n">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E33" s="53" t="n">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="34">
@@ -8433,13 +8433,13 @@
         <v>5</v>
       </c>
       <c r="C34" s="53" t="n">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D34" s="53" t="n">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E34" s="53" t="n">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="35">
@@ -8450,13 +8450,13 @@
         <v>5</v>
       </c>
       <c r="C35" s="53" t="n">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D35" s="53" t="n">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E35" s="53" t="n">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="36">
@@ -8467,13 +8467,13 @@
         <v>5</v>
       </c>
       <c r="C36" s="53" t="n">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D36" s="53" t="n">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E36" s="53" t="n">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="37">
@@ -8484,13 +8484,13 @@
         <v>5</v>
       </c>
       <c r="C37" s="53" t="n">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D37" s="53" t="n">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E37" s="53" t="n">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="38">
@@ -8501,13 +8501,13 @@
         <v>5</v>
       </c>
       <c r="C38" s="53" t="n">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D38" s="53" t="n">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E38" s="53" t="n">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="39">
@@ -8518,13 +8518,13 @@
         <v>5</v>
       </c>
       <c r="C39" s="53" t="n">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D39" s="53" t="n">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E39" s="53" t="n">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="40">
@@ -8535,13 +8535,13 @@
         <v>5</v>
       </c>
       <c r="C40" s="53" t="n">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D40" s="53" t="n">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E40" s="53" t="n">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="41">
@@ -8552,13 +8552,13 @@
         <v>5</v>
       </c>
       <c r="C41" s="53" t="n">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D41" s="53" t="n">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E41" s="53" t="n">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="42">
@@ -8569,13 +8569,13 @@
         <v>6</v>
       </c>
       <c r="C42" s="53" t="n">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D42" s="53" t="n">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E42" s="53" t="n">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="43">
@@ -8586,13 +8586,13 @@
         <v>7</v>
       </c>
       <c r="C43" s="53" t="n">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D43" s="53" t="n">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E43" s="53" t="n">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="44">
@@ -8603,13 +8603,13 @@
         <v>7</v>
       </c>
       <c r="C44" s="53" t="n">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="D44" s="53" t="n">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E44" s="53" t="n">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="45">
@@ -8620,13 +8620,13 @@
         <v>8</v>
       </c>
       <c r="C45" s="53" t="n">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D45" s="53" t="n">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E45" s="53" t="n">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="46">
@@ -8637,13 +8637,13 @@
         <v>8</v>
       </c>
       <c r="C46" s="53" t="n">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="D46" s="53" t="n">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="E46" s="53" t="n">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="47">
@@ -8654,13 +8654,13 @@
         <v>8</v>
       </c>
       <c r="C47" s="53" t="n">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D47" s="53" t="n">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="E47" s="53" t="n">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="48">
@@ -8671,13 +8671,13 @@
         <v>9</v>
       </c>
       <c r="C48" s="53" t="n">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D48" s="53" t="n">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="E48" s="53" t="n">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="49">
@@ -8688,13 +8688,13 @@
         <v>9</v>
       </c>
       <c r="C49" s="53" t="n">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D49" s="53" t="n">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="E49" s="53" t="n">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="50">
@@ -8705,13 +8705,13 @@
         <v>9</v>
       </c>
       <c r="C50" s="53" t="n">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="D50" s="53" t="n">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="E50" s="53" t="n">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="51">
@@ -8722,13 +8722,13 @@
         <v>9</v>
       </c>
       <c r="C51" s="53" t="n">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="D51" s="53" t="n">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E51" s="53" t="n">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="52">
@@ -8739,13 +8739,13 @@
         <v>9</v>
       </c>
       <c r="C52" s="53" t="n">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="D52" s="53" t="n">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="E52" s="53" t="n">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="53">
@@ -8756,13 +8756,13 @@
         <v>10</v>
       </c>
       <c r="C53" s="53" t="n">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="D53" s="53" t="n">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="E53" s="53" t="n">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="54">
@@ -8773,13 +8773,13 @@
         <v>10</v>
       </c>
       <c r="C54" s="53" t="n">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="D54" s="53" t="n">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E54" s="53" t="n">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="55">
@@ -8790,13 +8790,13 @@
         <v>10</v>
       </c>
       <c r="C55" s="53" t="n">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D55" s="53" t="n">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="E55" s="53" t="n">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="56">
@@ -8807,13 +8807,13 @@
         <v>11</v>
       </c>
       <c r="C56" s="53" t="n">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="D56" s="53" t="n">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="E56" s="53" t="n">
-        <v>732</v>
+        <v>733</v>
       </c>
     </row>
     <row r="57">
@@ -8824,13 +8824,13 @@
         <v>11</v>
       </c>
       <c r="C57" s="53" t="n">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="D57" s="53" t="n">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="E57" s="53" t="n">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="58">
@@ -8841,13 +8841,13 @@
         <v>11</v>
       </c>
       <c r="C58" s="53" t="n">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="D58" s="53" t="n">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="E58" s="53" t="n">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="59">
@@ -8858,13 +8858,13 @@
         <v>12</v>
       </c>
       <c r="C59" s="53" t="n">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="D59" s="53" t="n">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="E59" s="53" t="n">
-        <v>799</v>
+        <v>800</v>
       </c>
     </row>
     <row r="60">
@@ -8875,13 +8875,13 @@
         <v>12</v>
       </c>
       <c r="C60" s="53" t="n">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="D60" s="53" t="n">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="E60" s="53" t="n">
-        <v>821</v>
+        <v>822</v>
       </c>
     </row>
     <row r="61">
@@ -8892,13 +8892,13 @@
         <v>12</v>
       </c>
       <c r="C61" s="53" t="n">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="D61" s="53" t="n">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="E61" s="53" t="n">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="62">
@@ -8909,13 +8909,13 @@
         <v>12</v>
       </c>
       <c r="C62" s="53" t="n">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D62" s="53" t="n">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="E62" s="53" t="n">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="63">
@@ -8926,13 +8926,13 @@
         <v>12</v>
       </c>
       <c r="C63" s="53" t="n">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="D63" s="53" t="n">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="E63" s="53" t="n">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
     <row r="64">
@@ -8943,13 +8943,13 @@
         <v>12</v>
       </c>
       <c r="C64" s="53" t="n">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D64" s="53" t="n">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E64" s="53" t="n">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
     <row r="65">
@@ -8960,13 +8960,13 @@
         <v>12</v>
       </c>
       <c r="C65" s="53" t="n">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="D65" s="53" t="n">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="E65" s="53" t="n">
-        <v>864</v>
+        <v>865</v>
       </c>
     </row>
     <row r="66">
@@ -8977,13 +8977,13 @@
         <v>12</v>
       </c>
       <c r="C66" s="53" t="n">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="D66" s="53" t="n">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="E66" s="53" t="n">
-        <v>867</v>
+        <v>868</v>
       </c>
     </row>
     <row r="67">
@@ -8994,13 +8994,13 @@
         <v>13</v>
       </c>
       <c r="C67" s="53" t="n">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="D67" s="53" t="n">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="E67" s="53" t="n">
-        <v>872</v>
+        <v>873</v>
       </c>
     </row>
     <row r="68">
@@ -9011,13 +9011,13 @@
         <v>13</v>
       </c>
       <c r="C68" s="53" t="n">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="D68" s="53" t="n">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="E68" s="53" t="n">
-        <v>877</v>
+        <v>878</v>
       </c>
     </row>
     <row r="69">
@@ -9028,13 +9028,13 @@
         <v>13</v>
       </c>
       <c r="C69" s="53" t="n">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="D69" s="53" t="n">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="E69" s="53" t="n">
-        <v>882</v>
+        <v>883</v>
       </c>
     </row>
     <row r="70">
@@ -9045,13 +9045,13 @@
         <v>13</v>
       </c>
       <c r="C70" s="53" t="n">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D70" s="53" t="n">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="E70" s="53" t="n">
-        <v>885</v>
+        <v>886</v>
       </c>
     </row>
     <row r="71">
@@ -9062,13 +9062,13 @@
         <v>13</v>
       </c>
       <c r="C71" t="n">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="D71" t="n">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="E71" t="n">
-        <v>891</v>
+        <v>892</v>
       </c>
     </row>
   </sheetData>
@@ -9147,19 +9147,19 @@
         <v>3</v>
       </c>
       <c r="D2" s="53" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E2" s="53" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F2" s="53" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G2" s="53" t="n">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H2" s="53" t="n">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3">
@@ -9170,22 +9170,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="53" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D3" s="53" t="n">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E3" s="53" t="n">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="F3" s="53" t="n">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="G3" s="53" t="n">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="H3" s="53" t="n">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
@@ -9196,22 +9196,22 @@
         <v>1</v>
       </c>
       <c r="C4" s="53" t="n">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="D4" s="53" t="n">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E4" s="53" t="n">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F4" s="53" t="n">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G4" s="53" t="n">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="H4" s="53" t="n">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5">
@@ -9222,22 +9222,22 @@
         <v>1</v>
       </c>
       <c r="C5" s="53" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="D5" s="53" t="n">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="E5" s="53" t="n">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="F5" s="53" t="n">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="G5" s="53" t="n">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="H5" s="53" t="n">
-        <v>97</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6">
@@ -9248,22 +9248,22 @@
         <v>1</v>
       </c>
       <c r="C6" s="53" t="n">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="D6" s="53" t="n">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="E6" s="53" t="n">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="F6" s="53" t="n">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="G6" s="53" t="n">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="H6" s="53" t="n">
-        <v>116</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7">
@@ -9274,22 +9274,22 @@
         <v>1</v>
       </c>
       <c r="C7" s="53" t="n">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="D7" s="53" t="n">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="E7" s="53" t="n">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="F7" s="53" t="n">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="G7" s="53" t="n">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="H7" s="53" t="n">
-        <v>130</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8">
@@ -9300,22 +9300,22 @@
         <v>1</v>
       </c>
       <c r="C8" s="53" t="n">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="D8" s="53" t="n">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="E8" s="53" t="n">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="F8" s="53" t="n">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="G8" s="53" t="n">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="H8" s="53" t="n">
-        <v>145</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9">
@@ -9326,22 +9326,22 @@
         <v>1</v>
       </c>
       <c r="C9" s="53" t="n">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="D9" s="53" t="n">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="E9" s="53" t="n">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="F9" s="53" t="n">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="G9" s="53" t="n">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="H9" s="53" t="n">
-        <v>159</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10">
@@ -9352,22 +9352,22 @@
         <v>1</v>
       </c>
       <c r="C10" s="53" t="n">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="D10" s="53" t="n">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="E10" s="53" t="n">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="F10" s="53" t="n">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="G10" s="53" t="n">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="H10" s="53" t="n">
-        <v>185</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11">
@@ -9378,22 +9378,22 @@
         <v>2</v>
       </c>
       <c r="C11" s="53" t="n">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="D11" s="53" t="n">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="E11" s="53" t="n">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="F11" s="53" t="n">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="G11" s="53" t="n">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="H11" s="53" t="n">
-        <v>227</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12">
@@ -9404,22 +9404,22 @@
         <v>2</v>
       </c>
       <c r="C12" s="53" t="n">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="D12" s="53" t="n">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="E12" s="53" t="n">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="F12" s="53" t="n">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="G12" s="53" t="n">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="H12" s="53" t="n">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13">
@@ -9430,22 +9430,22 @@
         <v>2</v>
       </c>
       <c r="C13" s="53" t="n">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="D13" s="53" t="n">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="E13" s="53" t="n">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="F13" s="53" t="n">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="G13" s="53" t="n">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="H13" s="53" t="n">
-        <v>278</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14">
@@ -9456,22 +9456,22 @@
         <v>2</v>
       </c>
       <c r="C14" s="53" t="n">
-        <v>288</v>
+        <v>303</v>
       </c>
       <c r="D14" s="53" t="n">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="E14" s="53" t="n">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="F14" s="53" t="n">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="G14" s="53" t="n">
-        <v>299</v>
+        <v>314</v>
       </c>
       <c r="H14" s="53" t="n">
-        <v>302</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15">
@@ -9482,22 +9482,22 @@
         <v>3</v>
       </c>
       <c r="C15" s="53" t="n">
-        <v>324</v>
+        <v>339</v>
       </c>
       <c r="D15" s="53" t="n">
-        <v>327</v>
+        <v>342</v>
       </c>
       <c r="E15" s="53" t="n">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="F15" s="53" t="n">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="G15" s="53" t="n">
-        <v>334</v>
+        <v>349</v>
       </c>
       <c r="H15" s="53" t="n">
-        <v>336</v>
+        <v>351</v>
       </c>
     </row>
     <row r="16">
@@ -9508,22 +9508,22 @@
         <v>3</v>
       </c>
       <c r="C16" s="53" t="n">
-        <v>338</v>
+        <v>353</v>
       </c>
       <c r="D16" s="53" t="n">
-        <v>343</v>
+        <v>358</v>
       </c>
       <c r="E16" s="53" t="n">
-        <v>346</v>
+        <v>361</v>
       </c>
       <c r="F16" s="53" t="n">
-        <v>349</v>
+        <v>364</v>
       </c>
       <c r="G16" s="53" t="n">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="H16" s="53" t="n">
-        <v>352</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17">
@@ -9534,22 +9534,22 @@
         <v>3</v>
       </c>
       <c r="C17" s="53" t="n">
-        <v>358</v>
+        <v>373</v>
       </c>
       <c r="D17" s="53" t="n">
-        <v>366</v>
+        <v>381</v>
       </c>
       <c r="E17" s="53" t="n">
-        <v>374</v>
+        <v>389</v>
       </c>
       <c r="F17" s="53" t="n">
-        <v>382</v>
+        <v>397</v>
       </c>
       <c r="G17" s="53" t="n">
-        <v>383</v>
+        <v>398</v>
       </c>
       <c r="H17" s="53" t="n">
-        <v>391</v>
+        <v>406</v>
       </c>
     </row>
     <row r="18">
@@ -9560,22 +9560,22 @@
         <v>3</v>
       </c>
       <c r="C18" s="53" t="n">
-        <v>397</v>
+        <v>412</v>
       </c>
       <c r="D18" s="53" t="n">
-        <v>400</v>
+        <v>415</v>
       </c>
       <c r="E18" s="53" t="n">
-        <v>402</v>
+        <v>417</v>
       </c>
       <c r="F18" s="53" t="n">
-        <v>407</v>
+        <v>422</v>
       </c>
       <c r="G18" s="53" t="n">
-        <v>408</v>
+        <v>423</v>
       </c>
       <c r="H18" s="53" t="n">
-        <v>411</v>
+        <v>426</v>
       </c>
     </row>
     <row r="19">
@@ -9586,22 +9586,22 @@
         <v>3</v>
       </c>
       <c r="C19" s="53" t="n">
-        <v>415</v>
+        <v>430</v>
       </c>
       <c r="D19" s="53" t="n">
-        <v>425</v>
+        <v>440</v>
       </c>
       <c r="E19" s="53" t="n">
-        <v>430</v>
+        <v>445</v>
       </c>
       <c r="F19" s="53" t="n">
-        <v>438</v>
+        <v>453</v>
       </c>
       <c r="G19" s="53" t="n">
-        <v>439</v>
+        <v>454</v>
       </c>
       <c r="H19" s="53" t="n">
-        <v>444</v>
+        <v>459</v>
       </c>
     </row>
     <row r="20">
@@ -9612,22 +9612,22 @@
         <v>3</v>
       </c>
       <c r="C20" s="53" t="n">
-        <v>454</v>
+        <v>469</v>
       </c>
       <c r="D20" s="53" t="n">
-        <v>458</v>
+        <v>473</v>
       </c>
       <c r="E20" s="53" t="n">
-        <v>460</v>
+        <v>475</v>
       </c>
       <c r="F20" s="53" t="n">
-        <v>463</v>
+        <v>478</v>
       </c>
       <c r="G20" s="53" t="n">
-        <v>464</v>
+        <v>479</v>
       </c>
       <c r="H20" s="53" t="n">
-        <v>465</v>
+        <v>480</v>
       </c>
     </row>
     <row r="21">
@@ -9638,22 +9638,22 @@
         <v>3</v>
       </c>
       <c r="C21" s="53" t="n">
-        <v>469</v>
+        <v>484</v>
       </c>
       <c r="D21" s="53" t="n">
-        <v>474</v>
+        <v>489</v>
       </c>
       <c r="E21" s="53" t="n">
-        <v>480</v>
+        <v>495</v>
       </c>
       <c r="F21" s="53" t="n">
-        <v>483</v>
+        <v>498</v>
       </c>
       <c r="G21" s="53" t="n">
-        <v>484</v>
+        <v>499</v>
       </c>
       <c r="H21" s="53" t="n">
-        <v>488</v>
+        <v>503</v>
       </c>
     </row>
     <row r="22">
@@ -9664,22 +9664,22 @@
         <v>3</v>
       </c>
       <c r="C22" s="53" t="n">
-        <v>490</v>
+        <v>505</v>
       </c>
       <c r="D22" s="53" t="n">
-        <v>497</v>
+        <v>512</v>
       </c>
       <c r="E22" s="53" t="n">
-        <v>502</v>
+        <v>517</v>
       </c>
       <c r="F22" s="53" t="n">
-        <v>507</v>
+        <v>522</v>
       </c>
       <c r="G22" s="53" t="n">
-        <v>508</v>
+        <v>523</v>
       </c>
       <c r="H22" s="53" t="n">
-        <v>511</v>
+        <v>526</v>
       </c>
     </row>
     <row r="23">
@@ -9690,22 +9690,22 @@
         <v>3</v>
       </c>
       <c r="C23" s="53" t="n">
-        <v>515</v>
+        <v>530</v>
       </c>
       <c r="D23" s="53" t="n">
-        <v>522</v>
+        <v>537</v>
       </c>
       <c r="E23" s="53" t="n">
-        <v>526</v>
+        <v>541</v>
       </c>
       <c r="F23" s="53" t="n">
-        <v>529</v>
+        <v>544</v>
       </c>
       <c r="G23" s="53" t="n">
-        <v>530</v>
+        <v>545</v>
       </c>
       <c r="H23" s="53" t="n">
-        <v>533</v>
+        <v>548</v>
       </c>
     </row>
     <row r="24">
@@ -9716,22 +9716,22 @@
         <v>3</v>
       </c>
       <c r="C24" s="53" t="n">
-        <v>535</v>
+        <v>550</v>
       </c>
       <c r="D24" s="53" t="n">
-        <v>546</v>
+        <v>561</v>
       </c>
       <c r="E24" s="53" t="n">
-        <v>552</v>
+        <v>567</v>
       </c>
       <c r="F24" s="53" t="n">
-        <v>557</v>
+        <v>572</v>
       </c>
       <c r="G24" s="53" t="n">
-        <v>558</v>
+        <v>573</v>
       </c>
       <c r="H24" s="53" t="n">
-        <v>563</v>
+        <v>578</v>
       </c>
     </row>
     <row r="25">
@@ -9742,22 +9742,22 @@
         <v>3</v>
       </c>
       <c r="C25" s="53" t="n">
-        <v>565</v>
+        <v>580</v>
       </c>
       <c r="D25" s="53" t="n">
-        <v>569</v>
+        <v>584</v>
       </c>
       <c r="E25" s="53" t="n">
-        <v>572</v>
+        <v>587</v>
       </c>
       <c r="F25" s="53" t="n">
-        <v>579</v>
+        <v>594</v>
       </c>
       <c r="G25" s="53" t="n">
-        <v>580</v>
+        <v>595</v>
       </c>
       <c r="H25" s="53" t="n">
-        <v>581</v>
+        <v>596</v>
       </c>
     </row>
     <row r="26">
@@ -9768,22 +9768,22 @@
         <v>4</v>
       </c>
       <c r="C26" s="53" t="n">
-        <v>627</v>
+        <v>642</v>
       </c>
       <c r="D26" s="53" t="n">
-        <v>635</v>
+        <v>650</v>
       </c>
       <c r="E26" s="53" t="n">
-        <v>641</v>
+        <v>656</v>
       </c>
       <c r="F26" s="53" t="n">
-        <v>648</v>
+        <v>663</v>
       </c>
       <c r="G26" s="53" t="n">
-        <v>649</v>
+        <v>664</v>
       </c>
       <c r="H26" s="53" t="n">
-        <v>654</v>
+        <v>669</v>
       </c>
     </row>
     <row r="27">
@@ -9794,22 +9794,22 @@
         <v>4</v>
       </c>
       <c r="C27" s="53" t="n">
-        <v>656</v>
+        <v>671</v>
       </c>
       <c r="D27" s="53" t="n">
-        <v>660</v>
+        <v>675</v>
       </c>
       <c r="E27" s="53" t="n">
-        <v>663</v>
+        <v>678</v>
       </c>
       <c r="F27" s="53" t="n">
-        <v>669</v>
+        <v>684</v>
       </c>
       <c r="G27" s="53" t="n">
-        <v>670</v>
+        <v>685</v>
       </c>
       <c r="H27" s="53" t="n">
-        <v>673</v>
+        <v>688</v>
       </c>
     </row>
     <row r="28">
@@ -9820,22 +9820,22 @@
         <v>4</v>
       </c>
       <c r="C28" s="53" t="n">
-        <v>683</v>
+        <v>698</v>
       </c>
       <c r="D28" s="53" t="n">
-        <v>698</v>
+        <v>713</v>
       </c>
       <c r="E28" s="53" t="n">
-        <v>706</v>
+        <v>721</v>
       </c>
       <c r="F28" s="53" t="n">
-        <v>713</v>
+        <v>728</v>
       </c>
       <c r="G28" s="53" t="n">
-        <v>714</v>
+        <v>729</v>
       </c>
       <c r="H28" s="53" t="n">
-        <v>722</v>
+        <v>737</v>
       </c>
     </row>
     <row r="29">
@@ -9846,22 +9846,22 @@
         <v>4</v>
       </c>
       <c r="C29" s="53" t="n">
-        <v>724</v>
+        <v>739</v>
       </c>
       <c r="D29" s="53" t="n">
-        <v>731</v>
+        <v>746</v>
       </c>
       <c r="E29" s="53" t="n">
-        <v>734</v>
+        <v>749</v>
       </c>
       <c r="F29" s="53" t="n">
-        <v>737</v>
+        <v>752</v>
       </c>
       <c r="G29" s="53" t="n">
-        <v>738</v>
+        <v>753</v>
       </c>
       <c r="H29" s="53" t="n">
-        <v>742</v>
+        <v>757</v>
       </c>
     </row>
     <row r="30">
@@ -9872,22 +9872,22 @@
         <v>4</v>
       </c>
       <c r="C30" s="53" t="n">
-        <v>744</v>
+        <v>759</v>
       </c>
       <c r="D30" s="53" t="n">
-        <v>750</v>
+        <v>765</v>
       </c>
       <c r="E30" s="53" t="n">
-        <v>756</v>
+        <v>771</v>
       </c>
       <c r="F30" s="53" t="n">
-        <v>760</v>
+        <v>775</v>
       </c>
       <c r="G30" s="53" t="n">
-        <v>761</v>
+        <v>776</v>
       </c>
       <c r="H30" s="53" t="n">
-        <v>761</v>
+        <v>776</v>
       </c>
     </row>
     <row r="31">
@@ -9898,22 +9898,22 @@
         <v>5</v>
       </c>
       <c r="C31" s="53" t="n">
-        <v>763</v>
+        <v>778</v>
       </c>
       <c r="D31" s="53" t="n">
-        <v>774</v>
+        <v>789</v>
       </c>
       <c r="E31" s="53" t="n">
-        <v>778</v>
+        <v>793</v>
       </c>
       <c r="F31" s="53" t="n">
-        <v>784</v>
+        <v>799</v>
       </c>
       <c r="G31" s="53" t="n">
-        <v>785</v>
+        <v>800</v>
       </c>
       <c r="H31" s="53" t="n">
-        <v>790</v>
+        <v>805</v>
       </c>
     </row>
     <row r="32">
@@ -9924,22 +9924,22 @@
         <v>5</v>
       </c>
       <c r="C32" s="53" t="n">
-        <v>794</v>
+        <v>809</v>
       </c>
       <c r="D32" s="53" t="n">
-        <v>798</v>
+        <v>813</v>
       </c>
       <c r="E32" s="53" t="n">
-        <v>804</v>
+        <v>819</v>
       </c>
       <c r="F32" s="53" t="n">
-        <v>808</v>
+        <v>823</v>
       </c>
       <c r="G32" s="53" t="n">
-        <v>809</v>
+        <v>824</v>
       </c>
       <c r="H32" s="53" t="n">
-        <v>809</v>
+        <v>824</v>
       </c>
     </row>
     <row r="33">
@@ -9950,22 +9950,22 @@
         <v>5</v>
       </c>
       <c r="C33" s="53" t="n">
-        <v>811</v>
+        <v>826</v>
       </c>
       <c r="D33" s="53" t="n">
-        <v>819</v>
+        <v>834</v>
       </c>
       <c r="E33" s="53" t="n">
-        <v>828</v>
+        <v>843</v>
       </c>
       <c r="F33" s="53" t="n">
-        <v>837</v>
+        <v>852</v>
       </c>
       <c r="G33" s="53" t="n">
-        <v>838</v>
+        <v>853</v>
       </c>
       <c r="H33" s="53" t="n">
-        <v>838</v>
+        <v>853</v>
       </c>
     </row>
     <row r="34">
@@ -9976,22 +9976,22 @@
         <v>5</v>
       </c>
       <c r="C34" s="53" t="n">
-        <v>842</v>
+        <v>857</v>
       </c>
       <c r="D34" s="53" t="n">
-        <v>848</v>
+        <v>863</v>
       </c>
       <c r="E34" s="53" t="n">
-        <v>853</v>
+        <v>868</v>
       </c>
       <c r="F34" s="53" t="n">
-        <v>856</v>
+        <v>871</v>
       </c>
       <c r="G34" s="53" t="n">
-        <v>857</v>
+        <v>872</v>
       </c>
       <c r="H34" s="53" t="n">
-        <v>857</v>
+        <v>872</v>
       </c>
     </row>
     <row r="35">
@@ -10002,22 +10002,22 @@
         <v>5</v>
       </c>
       <c r="C35" s="53" t="n">
-        <v>865</v>
+        <v>880</v>
       </c>
       <c r="D35" s="53" t="n">
-        <v>872</v>
+        <v>887</v>
       </c>
       <c r="E35" s="53" t="n">
-        <v>876</v>
+        <v>891</v>
       </c>
       <c r="F35" s="53" t="n">
-        <v>880</v>
+        <v>895</v>
       </c>
       <c r="G35" s="53" t="n">
-        <v>881</v>
+        <v>896</v>
       </c>
       <c r="H35" s="53" t="n">
-        <v>889</v>
+        <v>904</v>
       </c>
     </row>
     <row r="36">
@@ -10028,22 +10028,22 @@
         <v>5</v>
       </c>
       <c r="C36" s="53" t="n">
-        <v>891</v>
+        <v>906</v>
       </c>
       <c r="D36" s="53" t="n">
-        <v>896</v>
+        <v>911</v>
       </c>
       <c r="E36" s="53" t="n">
-        <v>906</v>
+        <v>921</v>
       </c>
       <c r="F36" s="53" t="n">
-        <v>912</v>
+        <v>927</v>
       </c>
       <c r="G36" s="53" t="n">
-        <v>913</v>
+        <v>928</v>
       </c>
       <c r="H36" s="53" t="n">
-        <v>920</v>
+        <v>935</v>
       </c>
     </row>
     <row r="37">
@@ -10054,22 +10054,22 @@
         <v>5</v>
       </c>
       <c r="C37" s="53" t="n">
-        <v>922</v>
+        <v>937</v>
       </c>
       <c r="D37" s="53" t="n">
-        <v>927</v>
+        <v>942</v>
       </c>
       <c r="E37" s="53" t="n">
-        <v>932</v>
+        <v>947</v>
       </c>
       <c r="F37" s="53" t="n">
-        <v>938</v>
+        <v>953</v>
       </c>
       <c r="G37" s="53" t="n">
-        <v>939</v>
+        <v>954</v>
       </c>
       <c r="H37" s="53" t="n">
-        <v>946</v>
+        <v>961</v>
       </c>
     </row>
     <row r="38">
@@ -10080,22 +10080,22 @@
         <v>5</v>
       </c>
       <c r="C38" s="53" t="n">
-        <v>948</v>
+        <v>963</v>
       </c>
       <c r="D38" s="53" t="n">
-        <v>955</v>
+        <v>970</v>
       </c>
       <c r="E38" s="53" t="n">
-        <v>959</v>
+        <v>974</v>
       </c>
       <c r="F38" s="53" t="n">
-        <v>965</v>
+        <v>980</v>
       </c>
       <c r="G38" s="53" t="n">
-        <v>966</v>
+        <v>981</v>
       </c>
       <c r="H38" s="53" t="n">
-        <v>966</v>
+        <v>981</v>
       </c>
     </row>
     <row r="39">
@@ -10106,22 +10106,22 @@
         <v>5</v>
       </c>
       <c r="C39" s="53" t="n">
-        <v>984</v>
+        <v>999</v>
       </c>
       <c r="D39" s="53" t="n">
-        <v>988</v>
+        <v>1003</v>
       </c>
       <c r="E39" s="53" t="n">
-        <v>992</v>
+        <v>1007</v>
       </c>
       <c r="F39" s="53" t="n">
-        <v>995</v>
+        <v>1010</v>
       </c>
       <c r="G39" s="53" t="n">
-        <v>996</v>
+        <v>1011</v>
       </c>
       <c r="H39" s="53" t="n">
-        <v>998</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="40">
@@ -10132,22 +10132,22 @@
         <v>5</v>
       </c>
       <c r="C40" s="53" t="n">
-        <v>1006</v>
+        <v>1021</v>
       </c>
       <c r="D40" s="53" t="n">
-        <v>1012</v>
+        <v>1027</v>
       </c>
       <c r="E40" s="53" t="n">
-        <v>1016</v>
+        <v>1031</v>
       </c>
       <c r="F40" s="53" t="n">
-        <v>1022</v>
+        <v>1037</v>
       </c>
       <c r="G40" s="53" t="n">
-        <v>1023</v>
+        <v>1038</v>
       </c>
       <c r="H40" s="53" t="n">
-        <v>1023</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="41">
@@ -10158,22 +10158,22 @@
         <v>5</v>
       </c>
       <c r="C41" s="53" t="n">
-        <v>1031</v>
+        <v>1046</v>
       </c>
       <c r="D41" s="53" t="n">
-        <v>1034</v>
+        <v>1049</v>
       </c>
       <c r="E41" s="53" t="n">
-        <v>1037</v>
+        <v>1052</v>
       </c>
       <c r="F41" s="53" t="n">
-        <v>1040</v>
+        <v>1055</v>
       </c>
       <c r="G41" s="53" t="n">
-        <v>1041</v>
+        <v>1056</v>
       </c>
       <c r="H41" s="53" t="n">
-        <v>1043</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="42">
@@ -10184,22 +10184,22 @@
         <v>6</v>
       </c>
       <c r="C42" s="53" t="n">
-        <v>1047</v>
+        <v>1062</v>
       </c>
       <c r="D42" s="53" t="n">
-        <v>1054</v>
+        <v>1069</v>
       </c>
       <c r="E42" s="53" t="n">
-        <v>1059</v>
+        <v>1074</v>
       </c>
       <c r="F42" s="53" t="n">
-        <v>1063</v>
+        <v>1078</v>
       </c>
       <c r="G42" s="53" t="n">
-        <v>1064</v>
+        <v>1079</v>
       </c>
       <c r="H42" s="53" t="n">
-        <v>1066</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="43">
@@ -10210,22 +10210,22 @@
         <v>7</v>
       </c>
       <c r="C43" s="53" t="n">
-        <v>1148</v>
+        <v>1163</v>
       </c>
       <c r="D43" s="53" t="n">
-        <v>1153</v>
+        <v>1168</v>
       </c>
       <c r="E43" s="53" t="n">
-        <v>1156</v>
+        <v>1171</v>
       </c>
       <c r="F43" s="53" t="n">
-        <v>1160</v>
+        <v>1175</v>
       </c>
       <c r="G43" s="53" t="n">
-        <v>1161</v>
+        <v>1176</v>
       </c>
       <c r="H43" s="53" t="n">
-        <v>1164</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="44">
@@ -10236,22 +10236,22 @@
         <v>7</v>
       </c>
       <c r="C44" s="53" t="n">
-        <v>1196</v>
+        <v>1211</v>
       </c>
       <c r="D44" s="53" t="n">
-        <v>1205</v>
+        <v>1220</v>
       </c>
       <c r="E44" s="53" t="n">
-        <v>1211</v>
+        <v>1226</v>
       </c>
       <c r="F44" s="53" t="n">
-        <v>1216</v>
+        <v>1231</v>
       </c>
       <c r="G44" s="53" t="n">
-        <v>1217</v>
+        <v>1232</v>
       </c>
       <c r="H44" s="53" t="n">
-        <v>1221</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="45">
@@ -10262,22 +10262,22 @@
         <v>8</v>
       </c>
       <c r="C45" s="53" t="n">
-        <v>1269</v>
+        <v>1284</v>
       </c>
       <c r="D45" s="53" t="n">
-        <v>1273</v>
+        <v>1288</v>
       </c>
       <c r="E45" s="53" t="n">
-        <v>1277</v>
+        <v>1292</v>
       </c>
       <c r="F45" s="53" t="n">
-        <v>1282</v>
+        <v>1297</v>
       </c>
       <c r="G45" s="53" t="n">
-        <v>1283</v>
+        <v>1298</v>
       </c>
       <c r="H45" s="53" t="n">
-        <v>1284</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="46">
@@ -10288,22 +10288,22 @@
         <v>8</v>
       </c>
       <c r="C46" s="53" t="n">
-        <v>1292</v>
+        <v>1307</v>
       </c>
       <c r="D46" s="53" t="n">
-        <v>1298</v>
+        <v>1313</v>
       </c>
       <c r="E46" s="53" t="n">
-        <v>1302</v>
+        <v>1317</v>
       </c>
       <c r="F46" s="53" t="n">
-        <v>1312</v>
+        <v>1327</v>
       </c>
       <c r="G46" s="53" t="n">
-        <v>1313</v>
+        <v>1328</v>
       </c>
       <c r="H46" s="53" t="n">
-        <v>1313</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="47">
@@ -10314,22 +10314,22 @@
         <v>8</v>
       </c>
       <c r="C47" s="53" t="n">
-        <v>1319</v>
+        <v>1334</v>
       </c>
       <c r="D47" s="53" t="n">
-        <v>1328</v>
+        <v>1343</v>
       </c>
       <c r="E47" s="53" t="n">
-        <v>1333</v>
+        <v>1348</v>
       </c>
       <c r="F47" s="53" t="n">
-        <v>1337</v>
+        <v>1352</v>
       </c>
       <c r="G47" s="53" t="n">
-        <v>1338</v>
+        <v>1353</v>
       </c>
       <c r="H47" s="53" t="n">
-        <v>1341</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="48">
@@ -10340,22 +10340,22 @@
         <v>9</v>
       </c>
       <c r="C48" s="53" t="n">
-        <v>1343</v>
+        <v>1358</v>
       </c>
       <c r="D48" s="53" t="n">
-        <v>1346</v>
+        <v>1361</v>
       </c>
       <c r="E48" s="53" t="n">
-        <v>1350</v>
+        <v>1365</v>
       </c>
       <c r="F48" s="53" t="n">
-        <v>1355</v>
+        <v>1370</v>
       </c>
       <c r="G48" s="53" t="n">
-        <v>1356</v>
+        <v>1371</v>
       </c>
       <c r="H48" s="53" t="n">
-        <v>1358</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="49">
@@ -10366,22 +10366,22 @@
         <v>9</v>
       </c>
       <c r="C49" s="53" t="n">
-        <v>1376</v>
+        <v>1391</v>
       </c>
       <c r="D49" s="53" t="n">
-        <v>1382</v>
+        <v>1397</v>
       </c>
       <c r="E49" s="53" t="n">
-        <v>1386</v>
+        <v>1401</v>
       </c>
       <c r="F49" s="53" t="n">
-        <v>1396</v>
+        <v>1411</v>
       </c>
       <c r="G49" s="53" t="n">
-        <v>1397</v>
+        <v>1412</v>
       </c>
       <c r="H49" s="53" t="n">
-        <v>1402</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="50">
@@ -10392,22 +10392,22 @@
         <v>9</v>
       </c>
       <c r="C50" s="53" t="n">
-        <v>1422</v>
+        <v>1437</v>
       </c>
       <c r="D50" s="53" t="n">
-        <v>1430</v>
+        <v>1445</v>
       </c>
       <c r="E50" s="53" t="n">
-        <v>1435</v>
+        <v>1450</v>
       </c>
       <c r="F50" s="53" t="n">
-        <v>1441</v>
+        <v>1456</v>
       </c>
       <c r="G50" s="53" t="n">
-        <v>1442</v>
+        <v>1457</v>
       </c>
       <c r="H50" s="53" t="n">
-        <v>1447</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="51">
@@ -10418,22 +10418,22 @@
         <v>9</v>
       </c>
       <c r="C51" s="53" t="n">
-        <v>1455</v>
+        <v>1470</v>
       </c>
       <c r="D51" s="53" t="n">
-        <v>1465</v>
+        <v>1480</v>
       </c>
       <c r="E51" s="53" t="n">
-        <v>1472</v>
+        <v>1487</v>
       </c>
       <c r="F51" s="53" t="n">
-        <v>1479</v>
+        <v>1494</v>
       </c>
       <c r="G51" s="53" t="n">
-        <v>1480</v>
+        <v>1495</v>
       </c>
       <c r="H51" s="53" t="n">
-        <v>1480</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="52">
@@ -10444,22 +10444,22 @@
         <v>9</v>
       </c>
       <c r="C52" s="53" t="n">
-        <v>1484</v>
+        <v>1499</v>
       </c>
       <c r="D52" s="53" t="n">
-        <v>1490</v>
+        <v>1505</v>
       </c>
       <c r="E52" s="53" t="n">
-        <v>1495</v>
+        <v>1510</v>
       </c>
       <c r="F52" s="53" t="n">
-        <v>1503</v>
+        <v>1518</v>
       </c>
       <c r="G52" s="53" t="n">
-        <v>1504</v>
+        <v>1519</v>
       </c>
       <c r="H52" s="53" t="n">
-        <v>1508</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="53">
@@ -10470,22 +10470,22 @@
         <v>10</v>
       </c>
       <c r="C53" s="53" t="n">
-        <v>1520</v>
+        <v>1535</v>
       </c>
       <c r="D53" s="53" t="n">
-        <v>1526</v>
+        <v>1541</v>
       </c>
       <c r="E53" s="53" t="n">
-        <v>1531</v>
+        <v>1546</v>
       </c>
       <c r="F53" s="53" t="n">
-        <v>1536</v>
+        <v>1551</v>
       </c>
       <c r="G53" s="53" t="n">
-        <v>1537</v>
+        <v>1552</v>
       </c>
       <c r="H53" s="53" t="n">
-        <v>1540</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="54">
@@ -10496,22 +10496,22 @@
         <v>10</v>
       </c>
       <c r="C54" s="53" t="n">
-        <v>1568</v>
+        <v>1583</v>
       </c>
       <c r="D54" s="53" t="n">
-        <v>1573</v>
+        <v>1588</v>
       </c>
       <c r="E54" s="53" t="n">
-        <v>1578</v>
+        <v>1593</v>
       </c>
       <c r="F54" s="53" t="n">
-        <v>1583</v>
+        <v>1598</v>
       </c>
       <c r="G54" s="53" t="n">
-        <v>1584</v>
+        <v>1599</v>
       </c>
       <c r="H54" s="53" t="n">
-        <v>1588</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="55">
@@ -10522,22 +10522,22 @@
         <v>10</v>
       </c>
       <c r="C55" s="53" t="n">
-        <v>1616</v>
+        <v>1631</v>
       </c>
       <c r="D55" s="53" t="n">
-        <v>1620</v>
+        <v>1635</v>
       </c>
       <c r="E55" s="53" t="n">
-        <v>1622</v>
+        <v>1637</v>
       </c>
       <c r="F55" s="53" t="n">
-        <v>1626</v>
+        <v>1641</v>
       </c>
       <c r="G55" s="53" t="n">
-        <v>1627</v>
+        <v>1642</v>
       </c>
       <c r="H55" s="53" t="n">
-        <v>1627</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="56">
@@ -10548,22 +10548,22 @@
         <v>11</v>
       </c>
       <c r="C56" s="53" t="n">
-        <v>1636</v>
+        <v>1651</v>
       </c>
       <c r="D56" s="53" t="n">
-        <v>1645</v>
+        <v>1660</v>
       </c>
       <c r="E56" s="53" t="n">
-        <v>1651</v>
+        <v>1666</v>
       </c>
       <c r="F56" s="53" t="n">
-        <v>1659</v>
+        <v>1674</v>
       </c>
       <c r="G56" s="53" t="n">
-        <v>1660</v>
+        <v>1675</v>
       </c>
       <c r="H56" s="53" t="n">
-        <v>1665</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="57">
@@ -10574,22 +10574,22 @@
         <v>11</v>
       </c>
       <c r="C57" s="53" t="n">
-        <v>1669</v>
+        <v>1684</v>
       </c>
       <c r="D57" s="53" t="n">
-        <v>1675</v>
+        <v>1690</v>
       </c>
       <c r="E57" s="53" t="n">
-        <v>1680</v>
+        <v>1695</v>
       </c>
       <c r="F57" s="53" t="n">
-        <v>1688</v>
+        <v>1703</v>
       </c>
       <c r="G57" s="53" t="n">
-        <v>1689</v>
+        <v>1704</v>
       </c>
       <c r="H57" s="53" t="n">
-        <v>1694</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="58">
@@ -10600,22 +10600,22 @@
         <v>11</v>
       </c>
       <c r="C58" s="53" t="n">
-        <v>1724</v>
+        <v>1739</v>
       </c>
       <c r="D58" s="53" t="n">
-        <v>1727</v>
+        <v>1742</v>
       </c>
       <c r="E58" s="53" t="n">
-        <v>1729</v>
+        <v>1744</v>
       </c>
       <c r="F58" s="53" t="n">
-        <v>1732</v>
+        <v>1747</v>
       </c>
       <c r="G58" s="53" t="n">
-        <v>1733</v>
+        <v>1748</v>
       </c>
       <c r="H58" s="53" t="n">
-        <v>1734</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="59">
@@ -10626,22 +10626,22 @@
         <v>12</v>
       </c>
       <c r="C59" s="53" t="n">
-        <v>1760</v>
+        <v>1775</v>
       </c>
       <c r="D59" s="53" t="n">
-        <v>1762</v>
+        <v>1777</v>
       </c>
       <c r="E59" s="53" t="n">
-        <v>1765</v>
+        <v>1780</v>
       </c>
       <c r="F59" s="53" t="n">
-        <v>1770</v>
+        <v>1785</v>
       </c>
       <c r="G59" s="53" t="n">
-        <v>1771</v>
+        <v>1786</v>
       </c>
       <c r="H59" s="53" t="n">
-        <v>1773</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="60">
@@ -10652,22 +10652,22 @@
         <v>12</v>
       </c>
       <c r="C60" s="53" t="n">
-        <v>1793</v>
+        <v>1808</v>
       </c>
       <c r="D60" s="53" t="n">
-        <v>1800</v>
+        <v>1818</v>
       </c>
       <c r="E60" s="53" t="n">
-        <v>1803</v>
+        <v>1823</v>
       </c>
       <c r="F60" s="53" t="n">
-        <v>1808</v>
+        <v>1831</v>
       </c>
       <c r="G60" s="53" t="n">
-        <v>1809</v>
+        <v>1832</v>
       </c>
       <c r="H60" s="53" t="n">
-        <v>1811</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="61">
@@ -10678,22 +10678,22 @@
         <v>12</v>
       </c>
       <c r="C61" s="53" t="n">
-        <v>1819</v>
+        <v>1845</v>
       </c>
       <c r="D61" s="53" t="n">
-        <v>1824</v>
+        <v>1850</v>
       </c>
       <c r="E61" s="53" t="n">
-        <v>1827</v>
+        <v>1853</v>
       </c>
       <c r="F61" s="53" t="n">
-        <v>1830</v>
+        <v>1856</v>
       </c>
       <c r="G61" s="53" t="n">
-        <v>1831</v>
+        <v>1857</v>
       </c>
       <c r="H61" s="53" t="n">
-        <v>1833</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="62">
@@ -10704,22 +10704,22 @@
         <v>12</v>
       </c>
       <c r="C62" s="53" t="n">
-        <v>1849</v>
+        <v>1875</v>
       </c>
       <c r="D62" s="53" t="n">
-        <v>1853</v>
+        <v>1879</v>
       </c>
       <c r="E62" s="53" t="n">
-        <v>1857</v>
+        <v>1883</v>
       </c>
       <c r="F62" s="53" t="n">
-        <v>1860</v>
+        <v>1886</v>
       </c>
       <c r="G62" s="53" t="n">
-        <v>1861</v>
+        <v>1887</v>
       </c>
       <c r="H62" s="53" t="n">
-        <v>1864</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="63">
@@ -10730,22 +10730,22 @@
         <v>12</v>
       </c>
       <c r="C63" s="53" t="n">
-        <v>1866</v>
+        <v>1892</v>
       </c>
       <c r="D63" s="53" t="n">
-        <v>1870</v>
+        <v>1896</v>
       </c>
       <c r="E63" s="53" t="n">
-        <v>1872</v>
+        <v>1898</v>
       </c>
       <c r="F63" s="53" t="n">
-        <v>1875</v>
+        <v>1901</v>
       </c>
       <c r="G63" s="53" t="n">
-        <v>1876</v>
+        <v>1902</v>
       </c>
       <c r="H63" s="53" t="n">
-        <v>1877</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="64">
@@ -10756,22 +10756,22 @@
         <v>12</v>
       </c>
       <c r="C64" s="53" t="n">
-        <v>1881</v>
+        <v>1907</v>
       </c>
       <c r="D64" s="53" t="n">
-        <v>1884</v>
+        <v>1910</v>
       </c>
       <c r="E64" s="53" t="n">
-        <v>1887</v>
+        <v>1913</v>
       </c>
       <c r="F64" s="53" t="n">
-        <v>1891</v>
+        <v>1917</v>
       </c>
       <c r="G64" s="53" t="n">
-        <v>1892</v>
+        <v>1918</v>
       </c>
       <c r="H64" s="53" t="n">
-        <v>1894</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="65">
@@ -10782,22 +10782,22 @@
         <v>12</v>
       </c>
       <c r="C65" s="53" t="n">
-        <v>1896</v>
+        <v>1922</v>
       </c>
       <c r="D65" s="53" t="n">
-        <v>1899</v>
+        <v>1925</v>
       </c>
       <c r="E65" s="53" t="n">
-        <v>1901</v>
+        <v>1927</v>
       </c>
       <c r="F65" s="53" t="n">
-        <v>1904</v>
+        <v>1930</v>
       </c>
       <c r="G65" s="53" t="n">
-        <v>1905</v>
+        <v>1931</v>
       </c>
       <c r="H65" s="53" t="n">
-        <v>1906</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="66">
@@ -10808,22 +10808,22 @@
         <v>12</v>
       </c>
       <c r="C66" s="53" t="n">
-        <v>1908</v>
+        <v>1934</v>
       </c>
       <c r="D66" s="53" t="n">
-        <v>1911</v>
+        <v>1937</v>
       </c>
       <c r="E66" s="53" t="n">
-        <v>1914</v>
+        <v>1940</v>
       </c>
       <c r="F66" s="53" t="n">
-        <v>1917</v>
+        <v>1943</v>
       </c>
       <c r="G66" s="53" t="n">
-        <v>1918</v>
+        <v>1944</v>
       </c>
       <c r="H66" s="53" t="n">
-        <v>1920</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="67">
@@ -10834,22 +10834,22 @@
         <v>13</v>
       </c>
       <c r="C67" s="53" t="n">
-        <v>1922</v>
+        <v>1948</v>
       </c>
       <c r="D67" s="53" t="n">
-        <v>1926</v>
+        <v>1952</v>
       </c>
       <c r="E67" s="53" t="n">
-        <v>1930</v>
+        <v>1956</v>
       </c>
       <c r="F67" s="53" t="n">
-        <v>1935</v>
+        <v>1961</v>
       </c>
       <c r="G67" s="53" t="n">
-        <v>1936</v>
+        <v>1962</v>
       </c>
       <c r="H67" s="53" t="n">
-        <v>1939</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="68">
@@ -10860,22 +10860,22 @@
         <v>13</v>
       </c>
       <c r="C68" s="53" t="n">
-        <v>1941</v>
+        <v>1967</v>
       </c>
       <c r="D68" s="53" t="n">
-        <v>1944</v>
+        <v>1970</v>
       </c>
       <c r="E68" s="53" t="n">
-        <v>1947</v>
+        <v>1973</v>
       </c>
       <c r="F68" s="53" t="n">
-        <v>1949</v>
+        <v>1975</v>
       </c>
       <c r="G68" s="53" t="n">
-        <v>1950</v>
+        <v>1976</v>
       </c>
       <c r="H68" s="53" t="n">
-        <v>1952</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="69">
@@ -10886,22 +10886,22 @@
         <v>13</v>
       </c>
       <c r="C69" s="53" t="n">
-        <v>1954</v>
+        <v>1980</v>
       </c>
       <c r="D69" s="53" t="n">
-        <v>1961</v>
+        <v>1987</v>
       </c>
       <c r="E69" s="53" t="n">
-        <v>1966</v>
+        <v>1992</v>
       </c>
       <c r="F69" s="53" t="n">
-        <v>1973</v>
+        <v>1999</v>
       </c>
       <c r="G69" s="53" t="n">
-        <v>1974</v>
+        <v>2000</v>
       </c>
       <c r="H69" s="53" t="n">
-        <v>1980</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="70">
@@ -10912,22 +10912,22 @@
         <v>13</v>
       </c>
       <c r="C70" s="53" t="n">
-        <v>1982</v>
+        <v>2008</v>
       </c>
       <c r="D70" s="53" t="n">
-        <v>1986</v>
+        <v>2012</v>
       </c>
       <c r="E70" s="53" t="n">
-        <v>1989</v>
+        <v>2015</v>
       </c>
       <c r="F70" s="53" t="n">
-        <v>1992</v>
+        <v>2018</v>
       </c>
       <c r="G70" s="53" t="n">
-        <v>1993</v>
+        <v>2019</v>
       </c>
       <c r="H70" s="53" t="n">
-        <v>1995</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="71">
@@ -10938,22 +10938,22 @@
         <v>13</v>
       </c>
       <c r="C71" t="n">
-        <v>1999</v>
+        <v>2025</v>
       </c>
       <c r="D71" t="n">
-        <v>2002</v>
+        <v>2028</v>
       </c>
       <c r="E71" t="n">
-        <v>2004</v>
+        <v>2030</v>
       </c>
       <c r="F71" t="n">
-        <v>2006</v>
+        <v>2032</v>
       </c>
       <c r="G71" t="n">
-        <v>2007</v>
+        <v>2033</v>
       </c>
       <c r="H71" t="n">
-        <v>2009</v>
+        <v>2035</v>
       </c>
     </row>
   </sheetData>
@@ -11849,7 +11849,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
@@ -11962,7 +11962,7 @@
         <v>22</v>
       </c>
       <c r="E6" s="53" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -11973,13 +11973,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="53" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D7" s="53" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E7" s="53" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8">
@@ -11990,13 +11990,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="53" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D8" s="53" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E8" s="53" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9">
@@ -12007,13 +12007,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="53" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D9" s="53" t="n">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E9" s="53" t="n">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10">
@@ -12024,13 +12024,13 @@
         <v>3</v>
       </c>
       <c r="C10" s="53" t="n">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D10" s="53" t="n">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E10" s="53" t="n">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11">
@@ -12041,13 +12041,13 @@
         <v>3</v>
       </c>
       <c r="C11" s="53" t="n">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D11" s="53" t="n">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E11" s="53" t="n">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12">
@@ -12058,13 +12058,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="53" t="n">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D12" s="53" t="n">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E12" s="53" t="n">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13">
@@ -12075,13 +12075,13 @@
         <v>3</v>
       </c>
       <c r="C13" s="53" t="n">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="D13" s="53" t="n">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E13" s="53" t="n">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
@@ -12092,13 +12092,13 @@
         <v>4</v>
       </c>
       <c r="C14" s="53" t="n">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="D14" s="53" t="n">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="E14" s="53" t="n">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15">
@@ -12109,13 +12109,13 @@
         <v>4</v>
       </c>
       <c r="C15" s="53" t="n">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="D15" s="53" t="n">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="E15" s="53" t="n">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
@@ -12126,13 +12126,13 @@
         <v>4</v>
       </c>
       <c r="C16" s="53" t="n">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="D16" s="53" t="n">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E16" s="53" t="n">
-        <v>67</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17">
@@ -12143,13 +12143,13 @@
         <v>4</v>
       </c>
       <c r="C17" s="53" t="n">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D17" s="53" t="n">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E17" s="53" t="n">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18">
@@ -12160,13 +12160,13 @@
         <v>5</v>
       </c>
       <c r="C18" s="53" t="n">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="D18" s="53" t="n">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="E18" s="53" t="n">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19">
@@ -12177,13 +12177,13 @@
         <v>5</v>
       </c>
       <c r="C19" s="53" t="n">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D19" s="53" t="n">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="E19" s="53" t="n">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20">
@@ -12194,13 +12194,13 @@
         <v>5</v>
       </c>
       <c r="C20" s="53" t="n">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="D20" s="53" t="n">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="E20" s="53" t="n">
-        <v>87</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21">
@@ -12211,13 +12211,13 @@
         <v>5</v>
       </c>
       <c r="C21" s="53" t="n">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="D21" s="53" t="n">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="E21" s="53" t="n">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22">
@@ -12228,13 +12228,13 @@
         <v>6</v>
       </c>
       <c r="C22" s="53" t="n">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="D22" s="53" t="n">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="E22" s="53" t="n">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23">
@@ -12245,13 +12245,13 @@
         <v>6</v>
       </c>
       <c r="C23" s="53" t="n">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="D23" s="53" t="n">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="E23" s="53" t="n">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24">
@@ -12262,13 +12262,13 @@
         <v>6</v>
       </c>
       <c r="C24" s="53" t="n">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="D24" s="53" t="n">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="E24" s="53" t="n">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25">
@@ -12279,13 +12279,13 @@
         <v>6</v>
       </c>
       <c r="C25" s="53" t="n">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="D25" s="53" t="n">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="E25" s="53" t="n">
-        <v>110</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26">
@@ -12296,13 +12296,13 @@
         <v>9</v>
       </c>
       <c r="C26" s="53" t="n">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="D26" s="53" t="n">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="E26" s="53" t="n">
-        <v>113</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27">
@@ -12313,13 +12313,13 @@
         <v>9</v>
       </c>
       <c r="C27" s="53" t="n">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="D27" s="53" t="n">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="E27" s="53" t="n">
-        <v>117</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28">
@@ -12330,13 +12330,13 @@
         <v>10</v>
       </c>
       <c r="C28" s="53" t="n">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="D28" s="53" t="n">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="E28" s="53" t="n">
-        <v>122</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29">
@@ -12347,13 +12347,13 @@
         <v>10</v>
       </c>
       <c r="C29" s="53" t="n">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="D29" s="53" t="n">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="E29" s="53" t="n">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30">
@@ -12364,13 +12364,13 @@
         <v>10</v>
       </c>
       <c r="C30" s="53" t="n">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="D30" s="53" t="n">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="E30" s="53" t="n">
-        <v>130</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31">
@@ -12381,13 +12381,13 @@
         <v>10</v>
       </c>
       <c r="C31" s="53" t="n">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="D31" s="53" t="n">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="E31" s="53" t="n">
-        <v>135</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32">
@@ -12398,13 +12398,13 @@
         <v>11</v>
       </c>
       <c r="C32" s="53" t="n">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="D32" s="53" t="n">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="E32" s="53" t="n">
-        <v>139</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33">
@@ -12415,13 +12415,13 @@
         <v>11</v>
       </c>
       <c r="C33" s="53" t="n">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="D33" s="53" t="n">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="E33" s="53" t="n">
-        <v>146</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34">
@@ -12432,13 +12432,13 @@
         <v>11</v>
       </c>
       <c r="C34" s="53" t="n">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="D34" s="53" t="n">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="E34" s="53" t="n">
-        <v>151</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35">
@@ -12449,13 +12449,13 @@
         <v>11</v>
       </c>
       <c r="C35" s="53" t="n">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="D35" s="53" t="n">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="E35" s="53" t="n">
-        <v>156</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36">
@@ -12466,13 +12466,13 @@
         <v>12</v>
       </c>
       <c r="C36" s="53" t="n">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="D36" s="53" t="n">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="E36" s="53" t="n">
-        <v>161</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37">
@@ -12483,13 +12483,13 @@
         <v>12</v>
       </c>
       <c r="C37" s="53" t="n">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="D37" s="53" t="n">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="E37" s="53" t="n">
-        <v>166</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38">
@@ -12500,13 +12500,13 @@
         <v>12</v>
       </c>
       <c r="C38" s="53" t="n">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="D38" s="53" t="n">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="E38" s="53" t="n">
-        <v>171</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39">
@@ -12517,13 +12517,13 @@
         <v>12</v>
       </c>
       <c r="C39" s="53" t="n">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="D39" s="53" t="n">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="E39" s="53" t="n">
-        <v>177</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40">
@@ -12534,13 +12534,13 @@
         <v>13</v>
       </c>
       <c r="C40" s="53" t="n">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="D40" s="53" t="n">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="E40" s="53" t="n">
-        <v>184</v>
+        <v>197</v>
       </c>
     </row>
     <row r="41">
@@ -12551,13 +12551,13 @@
         <v>1</v>
       </c>
       <c r="C41" s="53" t="n">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="D41" s="53" t="n">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="E41" s="53" t="n">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42">
@@ -12568,13 +12568,13 @@
         <v>2</v>
       </c>
       <c r="C42" s="53" t="n">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="D42" s="53" t="n">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="E42" s="53" t="n">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43">
@@ -12585,13 +12585,13 @@
         <v>3</v>
       </c>
       <c r="C43" s="53" t="n">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="D43" s="53" t="n">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="E43" s="53" t="n">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44">
@@ -12602,13 +12602,13 @@
         <v>4</v>
       </c>
       <c r="C44" s="53" t="n">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="D44" s="53" t="n">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="E44" s="53" t="n">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="45">
@@ -12619,13 +12619,13 @@
         <v>5</v>
       </c>
       <c r="C45" s="53" t="n">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="D45" s="53" t="n">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="E45" s="53" t="n">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46">
@@ -12636,13 +12636,13 @@
         <v>6</v>
       </c>
       <c r="C46" s="53" t="n">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="D46" s="53" t="n">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="E46" s="53" t="n">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47">
@@ -12653,13 +12653,13 @@
         <v>9</v>
       </c>
       <c r="C47" s="53" t="n">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="D47" s="53" t="n">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="E47" s="53" t="n">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48">
@@ -12670,13 +12670,13 @@
         <v>10</v>
       </c>
       <c r="C48" s="53" t="n">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="D48" s="53" t="n">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="E48" s="53" t="n">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49">
@@ -12687,13 +12687,13 @@
         <v>11</v>
       </c>
       <c r="C49" s="53" t="n">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="D49" s="53" t="n">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="E49" s="53" t="n">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50">
@@ -12704,13 +12704,13 @@
         <v>12</v>
       </c>
       <c r="C50" s="53" t="n">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="D50" s="53" t="n">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="E50" s="53" t="n">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -14369,8 +14369,8 @@
     <col width="12.7109375" customWidth="1" style="6" min="17" max="17"/>
     <col width="13.85546875" customWidth="1" style="6" min="18" max="18"/>
     <col width="14.140625" customWidth="1" style="6" min="19" max="19"/>
-    <col width="9.140625" customWidth="1" style="6" min="20" max="29"/>
-    <col width="9.140625" customWidth="1" style="6" min="30" max="16384"/>
+    <col width="9.140625" customWidth="1" style="6" min="20" max="30"/>
+    <col width="9.140625" customWidth="1" style="6" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="54" customFormat="1" customHeight="1" s="47">

</xml_diff>